<commit_message>
calculation of new indicators
</commit_message>
<xml_diff>
--- a/scheme/Cadastro/issues_metadados_cadastro.xlsx
+++ b/scheme/Cadastro/issues_metadados_cadastro.xlsx
@@ -65404,7 +65404,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MQMS01</t>
+          <t>MQME001</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -65419,7 +65419,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MQMS02</t>
+          <t>MQME002</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -65434,7 +65434,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MQMS03</t>
+          <t>MQME003</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -65449,7 +65449,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>MQMS04</t>
+          <t>MQME004</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -65464,7 +65464,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>MQMS05</t>
+          <t>MQME005</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -65540,7 +65540,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MQME10</t>
+          <t>MQME012</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -65566,7 +65566,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -65596,7 +65596,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -65626,7 +65626,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -65656,7 +65656,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -65686,7 +65686,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -65716,7 +65716,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -65746,7 +65746,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -65776,7 +65776,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -65806,7 +65806,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -65836,7 +65836,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -65866,7 +65866,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -65896,7 +65896,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -65926,7 +65926,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -65956,7 +65956,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -65986,7 +65986,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -66016,7 +66016,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -66046,7 +66046,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -66076,7 +66076,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -66106,7 +66106,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -66136,7 +66136,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -66166,7 +66166,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -66196,7 +66196,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -66226,7 +66226,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -66256,7 +66256,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -66286,7 +66286,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -66316,7 +66316,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -66346,7 +66346,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -66376,7 +66376,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -66406,7 +66406,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -66436,7 +66436,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -66466,7 +66466,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -66496,7 +66496,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -66526,7 +66526,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -66556,7 +66556,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -66586,7 +66586,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -66616,7 +66616,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -66646,7 +66646,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -66676,7 +66676,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -66706,7 +66706,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -66736,7 +66736,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -66766,7 +66766,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -66796,7 +66796,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -66826,7 +66826,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -66856,7 +66856,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -66886,7 +66886,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -66916,7 +66916,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -66946,7 +66946,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -66976,7 +66976,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -67006,7 +67006,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -67036,7 +67036,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -67066,7 +67066,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -67096,7 +67096,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -67126,7 +67126,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -67156,7 +67156,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -67186,7 +67186,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -67216,7 +67216,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -67246,7 +67246,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -67276,7 +67276,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -67306,7 +67306,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -67336,7 +67336,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -67366,7 +67366,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -67396,7 +67396,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -67426,7 +67426,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -67456,7 +67456,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -67486,7 +67486,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -67516,7 +67516,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -67546,7 +67546,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -67576,7 +67576,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -67606,7 +67606,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -67636,7 +67636,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -67666,7 +67666,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -67696,7 +67696,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -67726,7 +67726,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -67756,7 +67756,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -67786,7 +67786,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -67816,7 +67816,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -67846,7 +67846,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -67876,7 +67876,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -67906,7 +67906,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -67936,7 +67936,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -67966,7 +67966,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -67996,7 +67996,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -68026,7 +68026,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -68056,7 +68056,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -68086,7 +68086,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -68116,7 +68116,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -68146,7 +68146,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -68176,7 +68176,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -68206,7 +68206,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -68236,7 +68236,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -68266,7 +68266,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -68296,7 +68296,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>MQME12</t>
+          <t>MQME014</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -68326,7 +68326,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -68356,7 +68356,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -68386,7 +68386,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -68416,7 +68416,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -68446,7 +68446,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -68476,7 +68476,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -68506,7 +68506,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -68536,7 +68536,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -68566,7 +68566,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -68596,7 +68596,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -68626,7 +68626,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -68656,7 +68656,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -68686,7 +68686,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -68716,7 +68716,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -68746,7 +68746,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -68776,7 +68776,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -68806,7 +68806,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -68836,7 +68836,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -68866,7 +68866,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -68896,7 +68896,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -68926,7 +68926,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -68956,7 +68956,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
@@ -68986,7 +68986,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -69016,7 +69016,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -69046,7 +69046,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -69076,7 +69076,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -69106,7 +69106,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -69136,7 +69136,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -69166,7 +69166,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -69196,7 +69196,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -69226,7 +69226,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -69256,7 +69256,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -69286,7 +69286,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -69316,7 +69316,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -69346,7 +69346,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -69376,7 +69376,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -69406,7 +69406,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -69436,7 +69436,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -69466,7 +69466,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -69496,7 +69496,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -69526,7 +69526,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -69556,7 +69556,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -69586,7 +69586,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -69616,7 +69616,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -69646,7 +69646,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
@@ -69676,7 +69676,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -69706,7 +69706,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -69736,7 +69736,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -69766,7 +69766,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -69796,7 +69796,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -69826,7 +69826,7 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
@@ -69856,7 +69856,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
@@ -69886,7 +69886,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -69916,7 +69916,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -69946,7 +69946,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
@@ -69976,7 +69976,7 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
@@ -70006,7 +70006,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -70036,7 +70036,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -70066,7 +70066,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -70096,7 +70096,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -70126,7 +70126,7 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
@@ -70156,7 +70156,7 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
@@ -70186,7 +70186,7 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
@@ -70216,7 +70216,7 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
@@ -70246,7 +70246,7 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
@@ -70276,7 +70276,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -70306,7 +70306,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -70336,7 +70336,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -70366,7 +70366,7 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
@@ -70396,7 +70396,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
@@ -70426,7 +70426,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -70456,7 +70456,7 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
@@ -70486,7 +70486,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
@@ -70516,7 +70516,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
@@ -70546,7 +70546,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
@@ -70576,7 +70576,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
@@ -70606,7 +70606,7 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
@@ -70636,7 +70636,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
@@ -70666,7 +70666,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
@@ -70696,7 +70696,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -70726,7 +70726,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -70756,7 +70756,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -70786,7 +70786,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -70816,7 +70816,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -70846,7 +70846,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
@@ -70876,7 +70876,7 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
@@ -70906,7 +70906,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
@@ -70936,7 +70936,7 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
@@ -70966,7 +70966,7 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
@@ -70996,7 +70996,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
@@ -71026,7 +71026,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
@@ -71056,7 +71056,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -71086,7 +71086,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -71116,7 +71116,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -71146,7 +71146,7 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
@@ -71176,7 +71176,7 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
@@ -71206,7 +71206,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
@@ -71236,7 +71236,7 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
@@ -71266,7 +71266,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
@@ -71296,7 +71296,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -71326,7 +71326,7 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
@@ -71356,7 +71356,7 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
@@ -71386,7 +71386,7 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
@@ -71416,7 +71416,7 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
@@ -71446,7 +71446,7 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
@@ -71476,7 +71476,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
@@ -71506,7 +71506,7 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
@@ -71536,7 +71536,7 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
@@ -71566,7 +71566,7 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
@@ -71596,7 +71596,7 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
@@ -71626,7 +71626,7 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
@@ -71656,7 +71656,7 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
@@ -71686,7 +71686,7 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
@@ -71716,7 +71716,7 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
@@ -71746,7 +71746,7 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
@@ -71776,7 +71776,7 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
@@ -71806,7 +71806,7 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
@@ -71836,7 +71836,7 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
@@ -71866,7 +71866,7 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
@@ -71896,7 +71896,7 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
@@ -71926,7 +71926,7 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
@@ -71956,7 +71956,7 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
@@ -71986,7 +71986,7 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
@@ -72016,7 +72016,7 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
@@ -72046,7 +72046,7 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
@@ -72076,7 +72076,7 @@
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
@@ -72106,7 +72106,7 @@
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
@@ -72136,7 +72136,7 @@
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
@@ -72166,7 +72166,7 @@
     <row r="223">
       <c r="A223" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B223" t="inlineStr">
@@ -72196,7 +72196,7 @@
     <row r="224">
       <c r="A224" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B224" t="inlineStr">
@@ -72226,7 +72226,7 @@
     <row r="225">
       <c r="A225" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B225" t="inlineStr">
@@ -72256,7 +72256,7 @@
     <row r="226">
       <c r="A226" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B226" t="inlineStr">
@@ -72286,7 +72286,7 @@
     <row r="227">
       <c r="A227" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B227" t="inlineStr">
@@ -72316,7 +72316,7 @@
     <row r="228">
       <c r="A228" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B228" t="inlineStr">
@@ -72346,7 +72346,7 @@
     <row r="229">
       <c r="A229" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B229" t="inlineStr">
@@ -72376,7 +72376,7 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
@@ -72406,7 +72406,7 @@
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
@@ -72436,7 +72436,7 @@
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
@@ -72466,7 +72466,7 @@
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
@@ -72496,7 +72496,7 @@
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
@@ -72526,7 +72526,7 @@
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
@@ -72556,7 +72556,7 @@
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
@@ -72586,7 +72586,7 @@
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
@@ -72616,7 +72616,7 @@
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
@@ -72646,7 +72646,7 @@
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
@@ -72676,7 +72676,7 @@
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
@@ -72706,7 +72706,7 @@
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
@@ -72736,7 +72736,7 @@
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
@@ -72766,7 +72766,7 @@
     <row r="243">
       <c r="A243" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B243" t="inlineStr">
@@ -72796,7 +72796,7 @@
     <row r="244">
       <c r="A244" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B244" t="inlineStr">
@@ -72826,7 +72826,7 @@
     <row r="245">
       <c r="A245" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B245" t="inlineStr">
@@ -72856,7 +72856,7 @@
     <row r="246">
       <c r="A246" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B246" t="inlineStr">
@@ -72886,7 +72886,7 @@
     <row r="247">
       <c r="A247" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B247" t="inlineStr">
@@ -72916,7 +72916,7 @@
     <row r="248">
       <c r="A248" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B248" t="inlineStr">
@@ -72946,7 +72946,7 @@
     <row r="249">
       <c r="A249" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B249" t="inlineStr">
@@ -72976,7 +72976,7 @@
     <row r="250">
       <c r="A250" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B250" t="inlineStr">
@@ -73006,7 +73006,7 @@
     <row r="251">
       <c r="A251" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B251" t="inlineStr">
@@ -73036,7 +73036,7 @@
     <row r="252">
       <c r="A252" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B252" t="inlineStr">
@@ -73066,7 +73066,7 @@
     <row r="253">
       <c r="A253" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B253" t="inlineStr">
@@ -73096,7 +73096,7 @@
     <row r="254">
       <c r="A254" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B254" t="inlineStr">
@@ -73126,7 +73126,7 @@
     <row r="255">
       <c r="A255" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B255" t="inlineStr">
@@ -73156,7 +73156,7 @@
     <row r="256">
       <c r="A256" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B256" t="inlineStr">
@@ -73186,7 +73186,7 @@
     <row r="257">
       <c r="A257" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B257" t="inlineStr">
@@ -73216,7 +73216,7 @@
     <row r="258">
       <c r="A258" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B258" t="inlineStr">
@@ -73246,7 +73246,7 @@
     <row r="259">
       <c r="A259" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B259" t="inlineStr">
@@ -73276,7 +73276,7 @@
     <row r="260">
       <c r="A260" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B260" t="inlineStr">
@@ -73306,7 +73306,7 @@
     <row r="261">
       <c r="A261" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B261" t="inlineStr">
@@ -73336,7 +73336,7 @@
     <row r="262">
       <c r="A262" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B262" t="inlineStr">
@@ -73366,7 +73366,7 @@
     <row r="263">
       <c r="A263" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B263" t="inlineStr">
@@ -73396,7 +73396,7 @@
     <row r="264">
       <c r="A264" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B264" t="inlineStr">
@@ -73426,7 +73426,7 @@
     <row r="265">
       <c r="A265" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B265" t="inlineStr">
@@ -73456,7 +73456,7 @@
     <row r="266">
       <c r="A266" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B266" t="inlineStr">
@@ -73486,7 +73486,7 @@
     <row r="267">
       <c r="A267" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B267" t="inlineStr">
@@ -73516,7 +73516,7 @@
     <row r="268">
       <c r="A268" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B268" t="inlineStr">
@@ -73546,7 +73546,7 @@
     <row r="269">
       <c r="A269" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B269" t="inlineStr">
@@ -73576,7 +73576,7 @@
     <row r="270">
       <c r="A270" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B270" t="inlineStr">
@@ -73606,7 +73606,7 @@
     <row r="271">
       <c r="A271" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B271" t="inlineStr">
@@ -73636,7 +73636,7 @@
     <row r="272">
       <c r="A272" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B272" t="inlineStr">
@@ -73666,7 +73666,7 @@
     <row r="273">
       <c r="A273" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B273" t="inlineStr">
@@ -73696,7 +73696,7 @@
     <row r="274">
       <c r="A274" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B274" t="inlineStr">
@@ -73726,7 +73726,7 @@
     <row r="275">
       <c r="A275" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B275" t="inlineStr">
@@ -73756,7 +73756,7 @@
     <row r="276">
       <c r="A276" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B276" t="inlineStr">
@@ -73786,7 +73786,7 @@
     <row r="277">
       <c r="A277" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B277" t="inlineStr">
@@ -73816,7 +73816,7 @@
     <row r="278">
       <c r="A278" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B278" t="inlineStr">
@@ -73846,7 +73846,7 @@
     <row r="279">
       <c r="A279" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B279" t="inlineStr">
@@ -73876,7 +73876,7 @@
     <row r="280">
       <c r="A280" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B280" t="inlineStr">
@@ -73906,7 +73906,7 @@
     <row r="281">
       <c r="A281" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B281" t="inlineStr">
@@ -73936,7 +73936,7 @@
     <row r="282">
       <c r="A282" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B282" t="inlineStr">
@@ -73966,7 +73966,7 @@
     <row r="283">
       <c r="A283" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B283" t="inlineStr">
@@ -73996,7 +73996,7 @@
     <row r="284">
       <c r="A284" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B284" t="inlineStr">
@@ -74026,7 +74026,7 @@
     <row r="285">
       <c r="A285" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B285" t="inlineStr">
@@ -74056,7 +74056,7 @@
     <row r="286">
       <c r="A286" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B286" t="inlineStr">
@@ -74086,7 +74086,7 @@
     <row r="287">
       <c r="A287" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B287" t="inlineStr">
@@ -74116,7 +74116,7 @@
     <row r="288">
       <c r="A288" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B288" t="inlineStr">
@@ -74146,7 +74146,7 @@
     <row r="289">
       <c r="A289" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B289" t="inlineStr">
@@ -74176,7 +74176,7 @@
     <row r="290">
       <c r="A290" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B290" t="inlineStr">
@@ -74206,7 +74206,7 @@
     <row r="291">
       <c r="A291" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B291" t="inlineStr">
@@ -74236,7 +74236,7 @@
     <row r="292">
       <c r="A292" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B292" t="inlineStr">
@@ -74266,7 +74266,7 @@
     <row r="293">
       <c r="A293" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B293" t="inlineStr">
@@ -74296,7 +74296,7 @@
     <row r="294">
       <c r="A294" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B294" t="inlineStr">
@@ -74326,7 +74326,7 @@
     <row r="295">
       <c r="A295" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B295" t="inlineStr">
@@ -74356,7 +74356,7 @@
     <row r="296">
       <c r="A296" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B296" t="inlineStr">
@@ -74386,7 +74386,7 @@
     <row r="297">
       <c r="A297" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B297" t="inlineStr">
@@ -74416,7 +74416,7 @@
     <row r="298">
       <c r="A298" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B298" t="inlineStr">
@@ -74446,7 +74446,7 @@
     <row r="299">
       <c r="A299" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B299" t="inlineStr">
@@ -74476,7 +74476,7 @@
     <row r="300">
       <c r="A300" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B300" t="inlineStr">
@@ -74506,7 +74506,7 @@
     <row r="301">
       <c r="A301" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B301" t="inlineStr">
@@ -74536,7 +74536,7 @@
     <row r="302">
       <c r="A302" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B302" t="inlineStr">
@@ -74566,7 +74566,7 @@
     <row r="303">
       <c r="A303" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B303" t="inlineStr">
@@ -74596,7 +74596,7 @@
     <row r="304">
       <c r="A304" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B304" t="inlineStr">
@@ -74626,7 +74626,7 @@
     <row r="305">
       <c r="A305" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B305" t="inlineStr">
@@ -74656,7 +74656,7 @@
     <row r="306">
       <c r="A306" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B306" t="inlineStr">
@@ -74686,7 +74686,7 @@
     <row r="307">
       <c r="A307" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B307" t="inlineStr">
@@ -74716,7 +74716,7 @@
     <row r="308">
       <c r="A308" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B308" t="inlineStr">
@@ -74746,7 +74746,7 @@
     <row r="309">
       <c r="A309" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B309" t="inlineStr">
@@ -74776,7 +74776,7 @@
     <row r="310">
       <c r="A310" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B310" t="inlineStr">
@@ -74806,7 +74806,7 @@
     <row r="311">
       <c r="A311" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B311" t="inlineStr">
@@ -74836,7 +74836,7 @@
     <row r="312">
       <c r="A312" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B312" t="inlineStr">
@@ -74866,7 +74866,7 @@
     <row r="313">
       <c r="A313" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B313" t="inlineStr">
@@ -74896,7 +74896,7 @@
     <row r="314">
       <c r="A314" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B314" t="inlineStr">
@@ -74926,7 +74926,7 @@
     <row r="315">
       <c r="A315" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B315" t="inlineStr">
@@ -74956,7 +74956,7 @@
     <row r="316">
       <c r="A316" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B316" t="inlineStr">
@@ -74986,7 +74986,7 @@
     <row r="317">
       <c r="A317" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B317" t="inlineStr">
@@ -75016,7 +75016,7 @@
     <row r="318">
       <c r="A318" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B318" t="inlineStr">
@@ -75046,7 +75046,7 @@
     <row r="319">
       <c r="A319" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B319" t="inlineStr">
@@ -75076,7 +75076,7 @@
     <row r="320">
       <c r="A320" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B320" t="inlineStr">
@@ -75106,7 +75106,7 @@
     <row r="321">
       <c r="A321" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B321" t="inlineStr">
@@ -75136,7 +75136,7 @@
     <row r="322">
       <c r="A322" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B322" t="inlineStr">
@@ -75166,7 +75166,7 @@
     <row r="323">
       <c r="A323" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B323" t="inlineStr">
@@ -75196,7 +75196,7 @@
     <row r="324">
       <c r="A324" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B324" t="inlineStr">
@@ -75226,7 +75226,7 @@
     <row r="325">
       <c r="A325" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B325" t="inlineStr">
@@ -75256,7 +75256,7 @@
     <row r="326">
       <c r="A326" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B326" t="inlineStr">
@@ -75286,7 +75286,7 @@
     <row r="327">
       <c r="A327" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B327" t="inlineStr">
@@ -75316,7 +75316,7 @@
     <row r="328">
       <c r="A328" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B328" t="inlineStr">
@@ -75346,7 +75346,7 @@
     <row r="329">
       <c r="A329" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B329" t="inlineStr">
@@ -75376,7 +75376,7 @@
     <row r="330">
       <c r="A330" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B330" t="inlineStr">
@@ -75406,7 +75406,7 @@
     <row r="331">
       <c r="A331" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B331" t="inlineStr">
@@ -75436,7 +75436,7 @@
     <row r="332">
       <c r="A332" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B332" t="inlineStr">
@@ -75466,7 +75466,7 @@
     <row r="333">
       <c r="A333" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B333" t="inlineStr">
@@ -75496,7 +75496,7 @@
     <row r="334">
       <c r="A334" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B334" t="inlineStr">
@@ -75526,7 +75526,7 @@
     <row r="335">
       <c r="A335" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B335" t="inlineStr">
@@ -75556,7 +75556,7 @@
     <row r="336">
       <c r="A336" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B336" t="inlineStr">
@@ -75586,7 +75586,7 @@
     <row r="337">
       <c r="A337" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B337" t="inlineStr">
@@ -75616,7 +75616,7 @@
     <row r="338">
       <c r="A338" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B338" t="inlineStr">
@@ -75646,7 +75646,7 @@
     <row r="339">
       <c r="A339" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B339" t="inlineStr">
@@ -75676,7 +75676,7 @@
     <row r="340">
       <c r="A340" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B340" t="inlineStr">
@@ -75706,7 +75706,7 @@
     <row r="341">
       <c r="A341" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B341" t="inlineStr">
@@ -75736,7 +75736,7 @@
     <row r="342">
       <c r="A342" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B342" t="inlineStr">
@@ -75766,7 +75766,7 @@
     <row r="343">
       <c r="A343" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B343" t="inlineStr">
@@ -75796,7 +75796,7 @@
     <row r="344">
       <c r="A344" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B344" t="inlineStr">
@@ -75826,7 +75826,7 @@
     <row r="345">
       <c r="A345" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B345" t="inlineStr">
@@ -75856,7 +75856,7 @@
     <row r="346">
       <c r="A346" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B346" t="inlineStr">
@@ -75886,7 +75886,7 @@
     <row r="347">
       <c r="A347" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B347" t="inlineStr">
@@ -75916,7 +75916,7 @@
     <row r="348">
       <c r="A348" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B348" t="inlineStr">
@@ -75946,7 +75946,7 @@
     <row r="349">
       <c r="A349" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B349" t="inlineStr">
@@ -75976,7 +75976,7 @@
     <row r="350">
       <c r="A350" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B350" t="inlineStr">
@@ -76006,7 +76006,7 @@
     <row r="351">
       <c r="A351" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B351" t="inlineStr">
@@ -76036,7 +76036,7 @@
     <row r="352">
       <c r="A352" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B352" t="inlineStr">
@@ -76066,7 +76066,7 @@
     <row r="353">
       <c r="A353" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B353" t="inlineStr">
@@ -76096,7 +76096,7 @@
     <row r="354">
       <c r="A354" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B354" t="inlineStr">
@@ -76126,7 +76126,7 @@
     <row r="355">
       <c r="A355" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B355" t="inlineStr">
@@ -76156,7 +76156,7 @@
     <row r="356">
       <c r="A356" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B356" t="inlineStr">
@@ -76186,7 +76186,7 @@
     <row r="357">
       <c r="A357" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B357" t="inlineStr">
@@ -76216,7 +76216,7 @@
     <row r="358">
       <c r="A358" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B358" t="inlineStr">
@@ -76246,7 +76246,7 @@
     <row r="359">
       <c r="A359" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B359" t="inlineStr">
@@ -76276,7 +76276,7 @@
     <row r="360">
       <c r="A360" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B360" t="inlineStr">
@@ -76306,7 +76306,7 @@
     <row r="361">
       <c r="A361" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B361" t="inlineStr">
@@ -76336,7 +76336,7 @@
     <row r="362">
       <c r="A362" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B362" t="inlineStr">
@@ -76366,7 +76366,7 @@
     <row r="363">
       <c r="A363" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B363" t="inlineStr">
@@ -76396,7 +76396,7 @@
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B364" t="inlineStr">
@@ -76426,7 +76426,7 @@
     <row r="365">
       <c r="A365" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B365" t="inlineStr">
@@ -76456,7 +76456,7 @@
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B366" t="inlineStr">
@@ -76486,7 +76486,7 @@
     <row r="367">
       <c r="A367" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B367" t="inlineStr">
@@ -76516,7 +76516,7 @@
     <row r="368">
       <c r="A368" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B368" t="inlineStr">
@@ -76546,7 +76546,7 @@
     <row r="369">
       <c r="A369" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B369" t="inlineStr">
@@ -76576,7 +76576,7 @@
     <row r="370">
       <c r="A370" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B370" t="inlineStr">
@@ -76606,7 +76606,7 @@
     <row r="371">
       <c r="A371" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B371" t="inlineStr">
@@ -76636,7 +76636,7 @@
     <row r="372">
       <c r="A372" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B372" t="inlineStr">
@@ -76666,7 +76666,7 @@
     <row r="373">
       <c r="A373" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B373" t="inlineStr">
@@ -76696,7 +76696,7 @@
     <row r="374">
       <c r="A374" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B374" t="inlineStr">
@@ -76726,7 +76726,7 @@
     <row r="375">
       <c r="A375" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B375" t="inlineStr">
@@ -76756,7 +76756,7 @@
     <row r="376">
       <c r="A376" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B376" t="inlineStr">
@@ -76786,7 +76786,7 @@
     <row r="377">
       <c r="A377" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B377" t="inlineStr">
@@ -76816,7 +76816,7 @@
     <row r="378">
       <c r="A378" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B378" t="inlineStr">
@@ -76846,7 +76846,7 @@
     <row r="379">
       <c r="A379" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B379" t="inlineStr">
@@ -76876,7 +76876,7 @@
     <row r="380">
       <c r="A380" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B380" t="inlineStr">
@@ -76906,7 +76906,7 @@
     <row r="381">
       <c r="A381" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B381" t="inlineStr">
@@ -76936,7 +76936,7 @@
     <row r="382">
       <c r="A382" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B382" t="inlineStr">
@@ -76966,7 +76966,7 @@
     <row r="383">
       <c r="A383" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B383" t="inlineStr">
@@ -76996,7 +76996,7 @@
     <row r="384">
       <c r="A384" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B384" t="inlineStr">
@@ -77026,7 +77026,7 @@
     <row r="385">
       <c r="A385" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B385" t="inlineStr">
@@ -77056,7 +77056,7 @@
     <row r="386">
       <c r="A386" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B386" t="inlineStr">
@@ -77086,7 +77086,7 @@
     <row r="387">
       <c r="A387" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B387" t="inlineStr">
@@ -77116,7 +77116,7 @@
     <row r="388">
       <c r="A388" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B388" t="inlineStr">
@@ -77146,7 +77146,7 @@
     <row r="389">
       <c r="A389" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B389" t="inlineStr">
@@ -77176,7 +77176,7 @@
     <row r="390">
       <c r="A390" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B390" t="inlineStr">
@@ -77206,7 +77206,7 @@
     <row r="391">
       <c r="A391" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B391" t="inlineStr">
@@ -77236,7 +77236,7 @@
     <row r="392">
       <c r="A392" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B392" t="inlineStr">
@@ -77266,7 +77266,7 @@
     <row r="393">
       <c r="A393" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B393" t="inlineStr">
@@ -77296,7 +77296,7 @@
     <row r="394">
       <c r="A394" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B394" t="inlineStr">
@@ -77326,7 +77326,7 @@
     <row r="395">
       <c r="A395" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B395" t="inlineStr">
@@ -77356,7 +77356,7 @@
     <row r="396">
       <c r="A396" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B396" t="inlineStr">
@@ -77386,7 +77386,7 @@
     <row r="397">
       <c r="A397" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B397" t="inlineStr">
@@ -77416,7 +77416,7 @@
     <row r="398">
       <c r="A398" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B398" t="inlineStr">
@@ -77446,7 +77446,7 @@
     <row r="399">
       <c r="A399" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B399" t="inlineStr">
@@ -77476,7 +77476,7 @@
     <row r="400">
       <c r="A400" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B400" t="inlineStr">
@@ -77506,7 +77506,7 @@
     <row r="401">
       <c r="A401" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B401" t="inlineStr">
@@ -77536,7 +77536,7 @@
     <row r="402">
       <c r="A402" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B402" t="inlineStr">
@@ -77566,7 +77566,7 @@
     <row r="403">
       <c r="A403" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B403" t="inlineStr">
@@ -77596,7 +77596,7 @@
     <row r="404">
       <c r="A404" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B404" t="inlineStr">
@@ -77626,7 +77626,7 @@
     <row r="405">
       <c r="A405" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B405" t="inlineStr">
@@ -77656,7 +77656,7 @@
     <row r="406">
       <c r="A406" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B406" t="inlineStr">
@@ -77686,7 +77686,7 @@
     <row r="407">
       <c r="A407" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B407" t="inlineStr">
@@ -77716,7 +77716,7 @@
     <row r="408">
       <c r="A408" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B408" t="inlineStr">
@@ -77746,7 +77746,7 @@
     <row r="409">
       <c r="A409" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B409" t="inlineStr">
@@ -77776,7 +77776,7 @@
     <row r="410">
       <c r="A410" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B410" t="inlineStr">
@@ -77806,7 +77806,7 @@
     <row r="411">
       <c r="A411" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B411" t="inlineStr">
@@ -77836,7 +77836,7 @@
     <row r="412">
       <c r="A412" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B412" t="inlineStr">
@@ -77866,7 +77866,7 @@
     <row r="413">
       <c r="A413" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B413" t="inlineStr">
@@ -77896,7 +77896,7 @@
     <row r="414">
       <c r="A414" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B414" t="inlineStr">
@@ -77926,7 +77926,7 @@
     <row r="415">
       <c r="A415" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B415" t="inlineStr">
@@ -77956,7 +77956,7 @@
     <row r="416">
       <c r="A416" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B416" t="inlineStr">
@@ -77986,7 +77986,7 @@
     <row r="417">
       <c r="A417" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B417" t="inlineStr">
@@ -78016,7 +78016,7 @@
     <row r="418">
       <c r="A418" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B418" t="inlineStr">
@@ -78046,7 +78046,7 @@
     <row r="419">
       <c r="A419" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B419" t="inlineStr">
@@ -78076,7 +78076,7 @@
     <row r="420">
       <c r="A420" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B420" t="inlineStr">
@@ -78106,7 +78106,7 @@
     <row r="421">
       <c r="A421" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B421" t="inlineStr">
@@ -78136,7 +78136,7 @@
     <row r="422">
       <c r="A422" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B422" t="inlineStr">
@@ -78166,7 +78166,7 @@
     <row r="423">
       <c r="A423" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B423" t="inlineStr">
@@ -78196,7 +78196,7 @@
     <row r="424">
       <c r="A424" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B424" t="inlineStr">
@@ -78226,7 +78226,7 @@
     <row r="425">
       <c r="A425" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B425" t="inlineStr">
@@ -78256,7 +78256,7 @@
     <row r="426">
       <c r="A426" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B426" t="inlineStr">
@@ -78286,7 +78286,7 @@
     <row r="427">
       <c r="A427" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B427" t="inlineStr">
@@ -78316,7 +78316,7 @@
     <row r="428">
       <c r="A428" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B428" t="inlineStr">
@@ -78346,7 +78346,7 @@
     <row r="429">
       <c r="A429" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B429" t="inlineStr">
@@ -78376,7 +78376,7 @@
     <row r="430">
       <c r="A430" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B430" t="inlineStr">
@@ -78406,7 +78406,7 @@
     <row r="431">
       <c r="A431" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B431" t="inlineStr">
@@ -78436,7 +78436,7 @@
     <row r="432">
       <c r="A432" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B432" t="inlineStr">
@@ -78466,7 +78466,7 @@
     <row r="433">
       <c r="A433" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B433" t="inlineStr">
@@ -78496,7 +78496,7 @@
     <row r="434">
       <c r="A434" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B434" t="inlineStr">
@@ -78526,7 +78526,7 @@
     <row r="435">
       <c r="A435" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B435" t="inlineStr">
@@ -78556,7 +78556,7 @@
     <row r="436">
       <c r="A436" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B436" t="inlineStr">
@@ -78586,7 +78586,7 @@
     <row r="437">
       <c r="A437" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B437" t="inlineStr">
@@ -78616,7 +78616,7 @@
     <row r="438">
       <c r="A438" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B438" t="inlineStr">
@@ -78646,7 +78646,7 @@
     <row r="439">
       <c r="A439" t="inlineStr">
         <is>
-          <t>MQME01</t>
+          <t>MQME008</t>
         </is>
       </c>
       <c r="B439" t="inlineStr">
@@ -78676,7 +78676,7 @@
     <row r="440">
       <c r="A440" t="inlineStr">
         <is>
-          <t>MQME14</t>
+          <t>MQME009</t>
         </is>
       </c>
       <c r="B440" t="inlineStr">
@@ -78710,7 +78710,7 @@
     <row r="441">
       <c r="A441" t="inlineStr">
         <is>
-          <t>MQME14</t>
+          <t>MQME009</t>
         </is>
       </c>
       <c r="B441" t="inlineStr">
@@ -78744,7 +78744,7 @@
     <row r="442">
       <c r="A442" t="inlineStr">
         <is>
-          <t>MQME14</t>
+          <t>MQME009</t>
         </is>
       </c>
       <c r="B442" t="inlineStr">
@@ -78778,7 +78778,7 @@
     <row r="443">
       <c r="A443" t="inlineStr">
         <is>
-          <t>MQME14</t>
+          <t>MQME009</t>
         </is>
       </c>
       <c r="B443" t="inlineStr">
@@ -78812,7 +78812,7 @@
     <row r="444">
       <c r="A444" t="inlineStr">
         <is>
-          <t>MQME14</t>
+          <t>MQME009</t>
         </is>
       </c>
       <c r="B444" t="inlineStr">
@@ -78846,7 +78846,7 @@
     <row r="445">
       <c r="A445" t="inlineStr">
         <is>
-          <t>MQME14</t>
+          <t>MQME009</t>
         </is>
       </c>
       <c r="B445" t="inlineStr">
@@ -78880,7 +78880,7 @@
     <row r="446">
       <c r="A446" t="inlineStr">
         <is>
-          <t>MQME14</t>
+          <t>MQME009</t>
         </is>
       </c>
       <c r="B446" t="inlineStr">
@@ -78914,7 +78914,7 @@
     <row r="447">
       <c r="A447" t="inlineStr">
         <is>
-          <t>MQME14</t>
+          <t>MQME009</t>
         </is>
       </c>
       <c r="B447" t="inlineStr">
@@ -78948,7 +78948,7 @@
     <row r="448">
       <c r="A448" t="inlineStr">
         <is>
-          <t>MQME14</t>
+          <t>MQME009</t>
         </is>
       </c>
       <c r="B448" t="inlineStr">
@@ -78982,7 +78982,7 @@
     <row r="449">
       <c r="A449" t="inlineStr">
         <is>
-          <t>MQME14</t>
+          <t>MQME009</t>
         </is>
       </c>
       <c r="B449" t="inlineStr">
@@ -79016,7 +79016,7 @@
     <row r="450">
       <c r="A450" t="inlineStr">
         <is>
-          <t>MQME14</t>
+          <t>MQME009</t>
         </is>
       </c>
       <c r="B450" t="inlineStr">
@@ -79050,7 +79050,7 @@
     <row r="451">
       <c r="A451" t="inlineStr">
         <is>
-          <t>MQME14</t>
+          <t>MQME009</t>
         </is>
       </c>
       <c r="B451" t="inlineStr">
@@ -79084,7 +79084,7 @@
     <row r="452">
       <c r="A452" t="inlineStr">
         <is>
-          <t>MQME14</t>
+          <t>MQME009</t>
         </is>
       </c>
       <c r="B452" t="inlineStr">
@@ -79118,7 +79118,7 @@
     <row r="453">
       <c r="A453" t="inlineStr">
         <is>
-          <t>MQME14</t>
+          <t>MQME009</t>
         </is>
       </c>
       <c r="B453" t="inlineStr">
@@ -79152,7 +79152,7 @@
     <row r="454">
       <c r="A454" t="inlineStr">
         <is>
-          <t>MQME14</t>
+          <t>MQME009</t>
         </is>
       </c>
       <c r="B454" t="inlineStr">
@@ -79186,7 +79186,7 @@
     <row r="455">
       <c r="A455" t="inlineStr">
         <is>
-          <t>MQME14</t>
+          <t>MQME009</t>
         </is>
       </c>
       <c r="B455" t="inlineStr">
@@ -79220,7 +79220,7 @@
     <row r="456">
       <c r="A456" t="inlineStr">
         <is>
-          <t>MQME14</t>
+          <t>MQME009</t>
         </is>
       </c>
       <c r="B456" t="inlineStr">
@@ -79254,7 +79254,7 @@
     <row r="457">
       <c r="A457" t="inlineStr">
         <is>
-          <t>MQME14</t>
+          <t>MQME009</t>
         </is>
       </c>
       <c r="B457" t="inlineStr">
@@ -79288,7 +79288,7 @@
     <row r="458">
       <c r="A458" t="inlineStr">
         <is>
-          <t>MQME14</t>
+          <t>MQME009</t>
         </is>
       </c>
       <c r="B458" t="inlineStr">
@@ -79322,7 +79322,7 @@
     <row r="459">
       <c r="A459" t="inlineStr">
         <is>
-          <t>MQME14</t>
+          <t>MQME009</t>
         </is>
       </c>
       <c r="B459" t="inlineStr">
@@ -79356,7 +79356,7 @@
     <row r="460">
       <c r="A460" t="inlineStr">
         <is>
-          <t>MQME14</t>
+          <t>MQME009</t>
         </is>
       </c>
       <c r="B460" t="inlineStr">
@@ -79390,7 +79390,7 @@
     <row r="461">
       <c r="A461" t="inlineStr">
         <is>
-          <t>MQME14</t>
+          <t>MQME009</t>
         </is>
       </c>
       <c r="B461" t="inlineStr">
@@ -79424,7 +79424,7 @@
     <row r="462">
       <c r="A462" t="inlineStr">
         <is>
-          <t>MQME14</t>
+          <t>MQME009</t>
         </is>
       </c>
       <c r="B462" t="inlineStr">
@@ -79458,7 +79458,7 @@
     <row r="463">
       <c r="A463" t="inlineStr">
         <is>
-          <t>MQME14</t>
+          <t>MQME009</t>
         </is>
       </c>
       <c r="B463" t="inlineStr">
@@ -79492,7 +79492,7 @@
     <row r="464">
       <c r="A464" t="inlineStr">
         <is>
-          <t>MQME14</t>
+          <t>MQME009</t>
         </is>
       </c>
       <c r="B464" t="inlineStr">
@@ -79526,7 +79526,7 @@
     <row r="465">
       <c r="A465" t="inlineStr">
         <is>
-          <t>MQME15</t>
+          <t>MQME010</t>
         </is>
       </c>
       <c r="B465" t="inlineStr">
@@ -79560,7 +79560,7 @@
     <row r="466">
       <c r="A466" t="inlineStr">
         <is>
-          <t>MQME15</t>
+          <t>MQME010</t>
         </is>
       </c>
       <c r="B466" t="inlineStr">
@@ -79594,7 +79594,7 @@
     <row r="467">
       <c r="A467" t="inlineStr">
         <is>
-          <t>MQME15</t>
+          <t>MQME010</t>
         </is>
       </c>
       <c r="B467" t="inlineStr">
@@ -79628,7 +79628,7 @@
     <row r="468">
       <c r="A468" t="inlineStr">
         <is>
-          <t>MQME15</t>
+          <t>MQME010</t>
         </is>
       </c>
       <c r="B468" t="inlineStr">
@@ -79662,7 +79662,7 @@
     <row r="469">
       <c r="A469" t="inlineStr">
         <is>
-          <t>MQME15</t>
+          <t>MQME010</t>
         </is>
       </c>
       <c r="B469" t="inlineStr">
@@ -79696,7 +79696,7 @@
     <row r="470">
       <c r="A470" t="inlineStr">
         <is>
-          <t>MQME15</t>
+          <t>MQME010</t>
         </is>
       </c>
       <c r="B470" t="inlineStr">
@@ -79730,7 +79730,7 @@
     <row r="471">
       <c r="A471" t="inlineStr">
         <is>
-          <t>MQME15</t>
+          <t>MQME010</t>
         </is>
       </c>
       <c r="B471" t="inlineStr">
@@ -79764,7 +79764,7 @@
     <row r="472">
       <c r="A472" t="inlineStr">
         <is>
-          <t>MQME15</t>
+          <t>MQME010</t>
         </is>
       </c>
       <c r="B472" t="inlineStr">
@@ -79798,7 +79798,7 @@
     <row r="473">
       <c r="A473" t="inlineStr">
         <is>
-          <t>MQME15</t>
+          <t>MQME010</t>
         </is>
       </c>
       <c r="B473" t="inlineStr">
@@ -79832,7 +79832,7 @@
     <row r="474">
       <c r="A474" t="inlineStr">
         <is>
-          <t>MQME15</t>
+          <t>MQME010</t>
         </is>
       </c>
       <c r="B474" t="inlineStr">
@@ -79866,7 +79866,7 @@
     <row r="475">
       <c r="A475" t="inlineStr">
         <is>
-          <t>MQME15</t>
+          <t>MQME010</t>
         </is>
       </c>
       <c r="B475" t="inlineStr">
@@ -79900,7 +79900,7 @@
     <row r="476">
       <c r="A476" t="inlineStr">
         <is>
-          <t>MQME15</t>
+          <t>MQME010</t>
         </is>
       </c>
       <c r="B476" t="inlineStr">
@@ -79934,7 +79934,7 @@
     <row r="477">
       <c r="A477" t="inlineStr">
         <is>
-          <t>MQME15</t>
+          <t>MQME010</t>
         </is>
       </c>
       <c r="B477" t="inlineStr">
@@ -79968,7 +79968,7 @@
     <row r="478">
       <c r="A478" t="inlineStr">
         <is>
-          <t>MQME15</t>
+          <t>MQME010</t>
         </is>
       </c>
       <c r="B478" t="inlineStr">
@@ -80002,7 +80002,7 @@
     <row r="479">
       <c r="A479" t="inlineStr">
         <is>
-          <t>MQME15</t>
+          <t>MQME010</t>
         </is>
       </c>
       <c r="B479" t="inlineStr">
@@ -80036,7 +80036,7 @@
     <row r="480">
       <c r="A480" t="inlineStr">
         <is>
-          <t>MQME15</t>
+          <t>MQME010</t>
         </is>
       </c>
       <c r="B480" t="inlineStr">
@@ -80070,7 +80070,7 @@
     <row r="481">
       <c r="A481" t="inlineStr">
         <is>
-          <t>MQME15</t>
+          <t>MQME010</t>
         </is>
       </c>
       <c r="B481" t="inlineStr">
@@ -80104,7 +80104,7 @@
     <row r="482">
       <c r="A482" t="inlineStr">
         <is>
-          <t>MQME15</t>
+          <t>MQME010</t>
         </is>
       </c>
       <c r="B482" t="inlineStr">
@@ -80138,7 +80138,7 @@
     <row r="483">
       <c r="A483" t="inlineStr">
         <is>
-          <t>MQME15</t>
+          <t>MQME010</t>
         </is>
       </c>
       <c r="B483" t="inlineStr">
@@ -80172,7 +80172,7 @@
     <row r="484">
       <c r="A484" t="inlineStr">
         <is>
-          <t>MQME15</t>
+          <t>MQME010</t>
         </is>
       </c>
       <c r="B484" t="inlineStr">
@@ -80206,7 +80206,7 @@
     <row r="485">
       <c r="A485" t="inlineStr">
         <is>
-          <t>MQME15</t>
+          <t>MQME010</t>
         </is>
       </c>
       <c r="B485" t="inlineStr">
@@ -80240,7 +80240,7 @@
     <row r="486">
       <c r="A486" t="inlineStr">
         <is>
-          <t>MQME15</t>
+          <t>MQME010</t>
         </is>
       </c>
       <c r="B486" t="inlineStr">
@@ -80274,7 +80274,7 @@
     <row r="487">
       <c r="A487" t="inlineStr">
         <is>
-          <t>MQME15</t>
+          <t>MQME010</t>
         </is>
       </c>
       <c r="B487" t="inlineStr">
@@ -80308,7 +80308,7 @@
     <row r="488">
       <c r="A488" t="inlineStr">
         <is>
-          <t>MQME15</t>
+          <t>MQME010</t>
         </is>
       </c>
       <c r="B488" t="inlineStr">
@@ -80342,7 +80342,7 @@
     <row r="489">
       <c r="A489" t="inlineStr">
         <is>
-          <t>MQME15</t>
+          <t>MQME010</t>
         </is>
       </c>
       <c r="B489" t="inlineStr">
@@ -80376,7 +80376,7 @@
     <row r="490">
       <c r="A490" t="inlineStr">
         <is>
-          <t>MQME15</t>
+          <t>MQME010</t>
         </is>
       </c>
       <c r="B490" t="inlineStr">
@@ -80418,7 +80418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -80446,45 +80446,30 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MQME00</t>
+          <t>MQME006</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Total number of columns</t>
+          <t>Total number of length-required columns</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1042</v>
+        <v>423</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MQMEA1</t>
+          <t>MQME007</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Total number of length-required columns</t>
+          <t>Total number of NUMBER columns</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>MQMEA2</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Total number of NUMBER columns</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
         <v>476</v>
       </c>
     </row>
@@ -80499,7 +80484,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -80527,29 +80512,29 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>IQME01</t>
+          <t>MQID001</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Columns with comments</t>
+          <t>Table names in singular</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>66.89%</t>
+          <t>98.89%</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>IQME02</t>
+          <t>MQID002</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Columns with data type</t>
+          <t>Table with recommended name length</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -80561,29 +80546,29 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>IQME03</t>
+          <t>MQID003</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Length-required columns with data length</t>
+          <t>Columns with correct prefixes</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>100.00%</t>
+          <t>91.17%</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>IQME04</t>
+          <t>MQID004</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>NUMBER columns with valid scale</t>
+          <t>Columns with recommended name size</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -80595,49 +80580,117 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>IQME05</t>
+          <t>MQID005</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Columns with valid num_distinct</t>
+          <t>Columns with comments</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>100.00%</t>
+          <t>66.89%</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>IQME06</t>
+          <t>MQID006</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Columns with valid num_nulls</t>
+          <t>Table with standard PK prefixes</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>100.00%</t>
+          <t>64.79%</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>IQME07</t>
+          <t>MQID007</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Columns with valid density</t>
+          <t>Table with standard FK prefixes</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
+        <is>
+          <t>61.19%</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>MQID008</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Table with standard UK prefixes</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>100.00%</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>MQID009</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>NUMBER columns with valid scale</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>100.00%</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>MQID010</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Columns with valid num_distinct</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>100.00%</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>MQID011</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Columns with valid num_nulls</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
         <is>
           <t>100.00%</t>
         </is>

</xml_diff>